<commit_message>
Fixes and changes - redid levels for alchemy
</commit_message>
<xml_diff>
--- a/resources/data-imports/items/Alchemy.xlsx
+++ b/resources/data-imports/items/Alchemy.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE558A5F-4D1A-C242-A492-B727E3078720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Items" sheetId="1" r:id="rId4"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -461,14 +478,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -483,21 +495,33 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -787,86 +811,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="M11" workbookViewId="0">
+      <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="507" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="27" max="27" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="28" max="28" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="30" max="30" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="31" max="31" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="32" max="32" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="33" max="33" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="34" max="34" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="35" max="35" width="29" bestFit="true" customWidth="true" style="0"/>
-    <col min="36" max="36" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="37" max="37" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="38" max="38" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="39" max="39" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="40" max="40" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="41" max="41" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="42" max="42" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="43" max="43" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="44" max="44" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="45" max="45" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="46" max="46" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="47" max="47" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="48" max="48" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="49" max="49" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="50" max="50" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="51" max="51" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="52" max="52" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="53" max="53" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="54" max="54" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="55" max="55" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="56" max="56" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="57" max="57" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="58" max="58" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="59" max="59" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="60" max="60" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="61" max="61" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="62" max="62" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="63" max="63" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="64" max="64" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="65" max="65" width="22" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="507" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="28" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="38" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="16" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="21" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="26" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="10" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="26" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1079,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:65">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>65596</v>
       </c>
@@ -1113,10 +1129,10 @@
         <v>1</v>
       </c>
       <c r="AR2">
-        <v>0.008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:65">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>65597</v>
       </c>
@@ -1169,7 +1185,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>65598</v>
       </c>
@@ -1225,7 +1241,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:65">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>65599</v>
       </c>
@@ -1281,7 +1297,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:65">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>65600</v>
       </c>
@@ -1337,7 +1353,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:65">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>65601</v>
       </c>
@@ -1393,7 +1409,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:65">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>65602</v>
       </c>
@@ -1431,7 +1447,7 @@
         <v>66</v>
       </c>
       <c r="AI8">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AL8">
         <v>1</v>
@@ -1449,7 +1465,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:65">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>65603</v>
       </c>
@@ -1499,7 +1515,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:65">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>65604</v>
       </c>
@@ -1552,7 +1568,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:65">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>65605</v>
       </c>
@@ -1608,7 +1624,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:65">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>65606</v>
       </c>
@@ -1646,7 +1662,7 @@
         <v>66</v>
       </c>
       <c r="AI12">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AL12">
         <v>1</v>
@@ -1664,7 +1680,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:65">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>65607</v>
       </c>
@@ -1717,7 +1733,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:65">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>65608</v>
       </c>
@@ -1773,7 +1789,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>65609</v>
       </c>
@@ -1829,7 +1845,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>65610</v>
       </c>
@@ -1885,36 +1901,33 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="17" spans="1:65">
+    <row r="17" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>65611</v>
+        <v>308797</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
         <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="K17">
-        <v>3000</v>
+        <v>2500</v>
       </c>
       <c r="L17">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="Y17">
         <v>1</v>
       </c>
-      <c r="Z17">
-        <v>1</v>
-      </c>
       <c r="AA17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="AB17">
         <v>70</v>
@@ -1925,37 +1938,34 @@
       <c r="AL17">
         <v>1</v>
       </c>
-      <c r="AM17">
-        <v>1</v>
-      </c>
-      <c r="AN17">
-        <v>1</v>
-      </c>
-      <c r="AO17">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="18" spans="1:65">
+      <c r="BG17">
+        <v>1</v>
+      </c>
+      <c r="BH17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>65612</v>
+        <v>65611</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" t="s">
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K18">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="L18">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="Y18">
         <v>1</v>
@@ -1964,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="AA18">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AB18">
         <v>70</v>
@@ -1978,37 +1988,34 @@
       <c r="AM18">
         <v>1</v>
       </c>
-      <c r="AP18">
-        <v>20</v>
-      </c>
-      <c r="AQ18">
-        <v>1</v>
-      </c>
-      <c r="AR18">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="19" spans="1:65">
+      <c r="AN18">
+        <v>1</v>
+      </c>
+      <c r="AO18">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>65613</v>
+        <v>65612</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
         <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K19">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="L19">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="Y19">
         <v>1</v>
@@ -2017,10 +2024,10 @@
         <v>1</v>
       </c>
       <c r="AA19">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="AB19">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AC19" t="s">
         <v>66</v>
@@ -2034,31 +2041,28 @@
       <c r="AP19">
         <v>20</v>
       </c>
-      <c r="AS19">
-        <v>4</v>
-      </c>
-      <c r="AT19">
-        <v>0.1</v>
-      </c>
-      <c r="AU19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:65">
+      <c r="AQ19">
+        <v>1</v>
+      </c>
+      <c r="AR19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>65614</v>
+        <v>65613</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
         <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="K20">
         <v>8000</v>
@@ -2081,9 +2085,6 @@
       <c r="AC20" t="s">
         <v>66</v>
       </c>
-      <c r="AI20">
-        <v>0.009</v>
-      </c>
       <c r="AL20">
         <v>1</v>
       </c>
@@ -2094,27 +2095,30 @@
         <v>20</v>
       </c>
       <c r="AS20">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="AT20">
+        <v>0.1</v>
       </c>
       <c r="AU20">
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:65">
+    <row r="21" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>65615</v>
+        <v>65614</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
         <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="K21">
         <v>8000</v>
@@ -2129,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="AA21">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="AB21">
         <v>80</v>
@@ -2137,6 +2141,9 @@
       <c r="AC21" t="s">
         <v>66</v>
       </c>
+      <c r="AI21">
+        <v>8.9999999999999993E-3</v>
+      </c>
       <c r="AL21">
         <v>1</v>
       </c>
@@ -2146,28 +2153,28 @@
       <c r="AP21">
         <v>20</v>
       </c>
-      <c r="AT21">
-        <v>0.01</v>
+      <c r="AS21">
+        <v>5</v>
       </c>
       <c r="AU21">
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:65">
+    <row r="22" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>65616</v>
+        <v>65615</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
         <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="K22">
         <v>8000</v>
@@ -2182,7 +2189,7 @@
         <v>1</v>
       </c>
       <c r="AA22">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AB22">
         <v>80</v>
@@ -2199,9 +2206,6 @@
       <c r="AP22">
         <v>20</v>
       </c>
-      <c r="AS22">
-        <v>1</v>
-      </c>
       <c r="AT22">
         <v>0.01</v>
       </c>
@@ -2209,21 +2213,21 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:65">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>65617</v>
+        <v>65616</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
         <v>66</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K23">
         <v>8000</v>
@@ -2238,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="AA23">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AB23">
         <v>80</v>
@@ -2256,7 +2260,7 @@
         <v>20</v>
       </c>
       <c r="AS23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT23">
         <v>0.01</v>
@@ -2265,21 +2269,21 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:65">
+    <row r="24" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>65618</v>
+        <v>65617</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" t="s">
         <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K24">
         <v>8000</v>
@@ -2294,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="AA24">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="AB24">
         <v>80</v>
@@ -2312,7 +2316,7 @@
         <v>20</v>
       </c>
       <c r="AS24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT24">
         <v>0.01</v>
@@ -2321,27 +2325,27 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:65">
+    <row r="25" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>65619</v>
+        <v>65618</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
         <v>66</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K25">
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="L25">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="Y25">
         <v>1</v>
@@ -2350,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="AA25">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="AB25">
         <v>80</v>
@@ -2364,14 +2368,20 @@
       <c r="AM25">
         <v>1</v>
       </c>
-      <c r="AN25">
-        <v>1</v>
-      </c>
-      <c r="AO25">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:65">
+      <c r="AP25">
+        <v>20</v>
+      </c>
+      <c r="AS25">
+        <v>3</v>
+      </c>
+      <c r="AT25">
+        <v>0.01</v>
+      </c>
+      <c r="AU25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>69935</v>
       </c>
@@ -2427,7 +2437,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:65">
+    <row r="27" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>69936</v>
       </c>
@@ -2495,7 +2505,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:65">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>69937</v>
       </c>
@@ -2557,27 +2567,27 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:65">
+    <row r="29" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>69938</v>
+        <v>65619</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
         <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="K29">
-        <v>21000</v>
+        <v>16000</v>
       </c>
       <c r="L29">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="Y29">
         <v>1</v>
@@ -2589,75 +2599,54 @@
         <v>50</v>
       </c>
       <c r="AB29">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AC29" t="s">
         <v>66</v>
       </c>
-      <c r="AF29">
-        <v>0.5</v>
-      </c>
-      <c r="AG29">
-        <v>0.5</v>
-      </c>
-      <c r="AH29">
-        <v>0.5</v>
-      </c>
-      <c r="AI29">
-        <v>0.5</v>
-      </c>
-      <c r="AJ29">
-        <v>0.5</v>
-      </c>
       <c r="AL29">
         <v>1</v>
       </c>
       <c r="AM29">
         <v>1</v>
       </c>
-      <c r="AP29">
-        <v>30</v>
-      </c>
-      <c r="AQ29">
-        <v>1</v>
-      </c>
-      <c r="AR29">
-        <v>0.15</v>
-      </c>
-      <c r="AT29">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:65">
+      <c r="AN29">
+        <v>1</v>
+      </c>
+      <c r="AO29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>155359</v>
+        <v>69938</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
         <v>66</v>
       </c>
       <c r="E30" t="s">
+        <v>108</v>
+      </c>
+      <c r="K30">
+        <v>21000</v>
+      </c>
+      <c r="L30">
         <v>110</v>
       </c>
-      <c r="K30">
-        <v>24000</v>
-      </c>
-      <c r="L30">
-        <v>120</v>
-      </c>
-      <c r="S30">
-        <v>0.35</v>
-      </c>
       <c r="Y30">
         <v>1</v>
       </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
       <c r="AA30">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AB30">
         <v>90</v>
@@ -2665,6 +2654,21 @@
       <c r="AC30" t="s">
         <v>66</v>
       </c>
+      <c r="AF30">
+        <v>0.5</v>
+      </c>
+      <c r="AG30">
+        <v>0.5</v>
+      </c>
+      <c r="AH30">
+        <v>0.5</v>
+      </c>
+      <c r="AI30">
+        <v>0.5</v>
+      </c>
+      <c r="AJ30">
+        <v>0.5</v>
+      </c>
       <c r="AL30">
         <v>1</v>
       </c>
@@ -2672,42 +2676,45 @@
         <v>1</v>
       </c>
       <c r="AP30">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AQ30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:65">
+      <c r="AR30">
+        <v>0.15</v>
+      </c>
+      <c r="AT30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>155360</v>
+        <v>308798</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D31" t="s">
         <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="K31">
-        <v>24000</v>
+        <v>21000</v>
       </c>
       <c r="L31">
-        <v>120</v>
-      </c>
-      <c r="U31">
-        <v>0.35</v>
+        <v>110</v>
       </c>
       <c r="Y31">
         <v>1</v>
       </c>
       <c r="AA31">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB31">
         <v>90</v>
@@ -2718,31 +2725,28 @@
       <c r="AL31">
         <v>1</v>
       </c>
-      <c r="AM31">
-        <v>1</v>
-      </c>
-      <c r="AP31">
-        <v>15</v>
-      </c>
-      <c r="AQ31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:65">
+      <c r="BG31">
+        <v>1</v>
+      </c>
+      <c r="BH31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>155362</v>
+        <v>155359</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
         <v>66</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K32">
         <v>24000</v>
@@ -2750,7 +2754,7 @@
       <c r="L32">
         <v>120</v>
       </c>
-      <c r="T32">
+      <c r="S32">
         <v>0.35</v>
       </c>
       <c r="Y32">
@@ -2778,21 +2782,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:65">
+    <row r="33" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>155363</v>
+        <v>155360</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
         <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="K33">
         <v>24000</v>
@@ -2800,14 +2804,14 @@
       <c r="L33">
         <v>120</v>
       </c>
-      <c r="W33">
+      <c r="U33">
         <v>0.35</v>
       </c>
       <c r="Y33">
         <v>1</v>
       </c>
       <c r="AA33">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AB33">
         <v>90</v>
@@ -2828,21 +2832,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:65">
+    <row r="34" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>155364</v>
+        <v>155362</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D34" t="s">
         <v>66</v>
       </c>
       <c r="E34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K34">
         <v>24000</v>
@@ -2850,14 +2854,14 @@
       <c r="L34">
         <v>120</v>
       </c>
-      <c r="V34">
+      <c r="T34">
         <v>0.35</v>
       </c>
       <c r="Y34">
         <v>1</v>
       </c>
       <c r="AA34">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="AB34">
         <v>90</v>
@@ -2878,33 +2882,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:65">
+    <row r="35" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>155365</v>
+        <v>155363</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
         <v>66</v>
       </c>
       <c r="E35" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35">
+        <v>24000</v>
+      </c>
+      <c r="L35">
         <v>120</v>
       </c>
-      <c r="K35">
-        <v>25000</v>
-      </c>
-      <c r="L35">
-        <v>128</v>
+      <c r="W35">
+        <v>0.35</v>
       </c>
       <c r="Y35">
         <v>1</v>
       </c>
       <c r="AA35">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AB35">
         <v>90</v>
@@ -2912,64 +2919,49 @@
       <c r="AC35" t="s">
         <v>66</v>
       </c>
-      <c r="AF35">
+      <c r="AL35">
+        <v>1</v>
+      </c>
+      <c r="AM35">
+        <v>1</v>
+      </c>
+      <c r="AP35">
+        <v>15</v>
+      </c>
+      <c r="AQ35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>155364</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>118</v>
+      </c>
+      <c r="K36">
+        <v>24000</v>
+      </c>
+      <c r="L36">
+        <v>120</v>
+      </c>
+      <c r="V36">
         <v>0.35</v>
       </c>
-      <c r="AG35">
-        <v>0.35</v>
-      </c>
-      <c r="AH35">
-        <v>0.35</v>
-      </c>
-      <c r="AL35">
-        <v>1</v>
-      </c>
-      <c r="AM35">
-        <v>1</v>
-      </c>
-      <c r="AP35">
-        <v>30</v>
-      </c>
-      <c r="AQ35">
-        <v>1</v>
-      </c>
-      <c r="AR35">
-        <v>0.6</v>
-      </c>
-      <c r="AT35">
-        <v>0.2</v>
-      </c>
-      <c r="AU35">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:65">
-      <c r="A36">
-        <v>155366</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>121</v>
-      </c>
-      <c r="D36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E36" t="s">
-        <v>122</v>
-      </c>
-      <c r="K36">
-        <v>28000</v>
-      </c>
-      <c r="L36">
-        <v>130</v>
-      </c>
       <c r="Y36">
         <v>1</v>
       </c>
       <c r="AA36">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="AB36">
         <v>90</v>
@@ -2977,9 +2969,6 @@
       <c r="AC36" t="s">
         <v>66</v>
       </c>
-      <c r="AH36">
-        <v>0.75</v>
-      </c>
       <c r="AL36">
         <v>1</v>
       </c>
@@ -2987,45 +2976,42 @@
         <v>1</v>
       </c>
       <c r="AP36">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:65">
+        <v>15</v>
+      </c>
+      <c r="AQ36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>155367</v>
+        <v>308036</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D37" t="s">
         <v>66</v>
       </c>
       <c r="E37" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="K37">
-        <v>28000</v>
+        <v>24000</v>
       </c>
       <c r="L37">
-        <v>130</v>
-      </c>
-      <c r="T37">
-        <v>0.75</v>
-      </c>
-      <c r="U37">
-        <v>0.75</v>
-      </c>
-      <c r="W37">
-        <v>0.75</v>
+        <v>120</v>
+      </c>
+      <c r="R37">
+        <v>0.35</v>
       </c>
       <c r="Y37">
         <v>1</v>
       </c>
       <c r="AA37">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="AB37">
         <v>90</v>
@@ -3033,9 +3019,6 @@
       <c r="AC37" t="s">
         <v>66</v>
       </c>
-      <c r="AF37">
-        <v>0.75</v>
-      </c>
       <c r="AL37">
         <v>1</v>
       </c>
@@ -3043,57 +3026,54 @@
         <v>1</v>
       </c>
       <c r="AP37">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AQ37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:65">
+    <row r="38" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>155368</v>
+        <v>155365</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D38" t="s">
         <v>66</v>
       </c>
       <c r="E38" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="K38">
-        <v>28000</v>
+        <v>25000</v>
       </c>
       <c r="L38">
-        <v>130</v>
-      </c>
-      <c r="Q38">
-        <v>0.75</v>
-      </c>
-      <c r="R38">
-        <v>0.75</v>
-      </c>
-      <c r="S38">
-        <v>0.75</v>
+        <v>128</v>
       </c>
       <c r="Y38">
         <v>1</v>
       </c>
       <c r="AA38">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="AB38">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="AC38" t="s">
         <v>66</v>
       </c>
       <c r="AF38">
-        <v>0.75</v>
+        <v>0.35</v>
+      </c>
+      <c r="AG38">
+        <v>0.35</v>
+      </c>
+      <c r="AH38">
+        <v>0.35</v>
       </c>
       <c r="AL38">
         <v>1</v>
@@ -3104,22 +3084,34 @@
       <c r="AP38">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="1:65">
+      <c r="AQ38">
+        <v>1</v>
+      </c>
+      <c r="AR38">
+        <v>0.6</v>
+      </c>
+      <c r="AT38">
+        <v>0.2</v>
+      </c>
+      <c r="AU38">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>155369</v>
+        <v>155367</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D39" t="s">
         <v>66</v>
       </c>
       <c r="E39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K39">
         <v>28000</v>
@@ -3127,20 +3119,23 @@
       <c r="L39">
         <v>130</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <v>0.75</v>
       </c>
-      <c r="V39">
+      <c r="U39">
         <v>0.75</v>
       </c>
+      <c r="W39">
+        <v>0.75</v>
+      </c>
       <c r="Y39">
         <v>1</v>
       </c>
       <c r="AA39">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="AB39">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="AC39" t="s">
         <v>66</v>
@@ -3157,37 +3152,37 @@
       <c r="AP39">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:65">
+      <c r="AQ39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>308036</v>
+        <v>155366</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
         <v>66</v>
       </c>
       <c r="E40" t="s">
+        <v>122</v>
+      </c>
+      <c r="K40">
+        <v>28000</v>
+      </c>
+      <c r="L40">
         <v>130</v>
       </c>
-      <c r="K40">
-        <v>24000</v>
-      </c>
-      <c r="L40">
-        <v>120</v>
-      </c>
-      <c r="R40">
-        <v>0.35</v>
-      </c>
       <c r="Y40">
         <v>1</v>
       </c>
       <c r="AA40">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AB40">
         <v>90</v>
@@ -3195,6 +3190,9 @@
       <c r="AC40" t="s">
         <v>66</v>
       </c>
+      <c r="AH40">
+        <v>0.75</v>
+      </c>
       <c r="AL40">
         <v>1</v>
       </c>
@@ -3202,21 +3200,18 @@
         <v>1</v>
       </c>
       <c r="AP40">
-        <v>15</v>
-      </c>
-      <c r="AQ40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>308797</v>
+        <v>308799</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D41" t="s">
         <v>66</v>
@@ -3225,19 +3220,19 @@
         <v>132</v>
       </c>
       <c r="K41">
-        <v>2500</v>
+        <v>28000</v>
       </c>
       <c r="L41">
-        <v>24</v>
+        <v>130</v>
       </c>
       <c r="Y41">
         <v>1</v>
       </c>
       <c r="AA41">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="AB41">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="AC41" t="s">
         <v>66</v>
@@ -3249,68 +3244,80 @@
         <v>1</v>
       </c>
       <c r="BH41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>308798</v>
+        <v>155368</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D42" t="s">
         <v>66</v>
       </c>
       <c r="E42" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="K42">
-        <v>21000</v>
+        <v>28000</v>
       </c>
       <c r="L42">
-        <v>110</v>
+        <v>130</v>
+      </c>
+      <c r="Q42">
+        <v>0.75</v>
+      </c>
+      <c r="R42">
+        <v>0.75</v>
+      </c>
+      <c r="S42">
+        <v>0.75</v>
       </c>
       <c r="Y42">
         <v>1</v>
       </c>
       <c r="AA42">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AB42">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="AC42" t="s">
         <v>66</v>
       </c>
+      <c r="AF42">
+        <v>0.75</v>
+      </c>
       <c r="AL42">
         <v>1</v>
       </c>
-      <c r="BG42">
-        <v>1</v>
-      </c>
-      <c r="BH42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:65">
+      <c r="AM42">
+        <v>1</v>
+      </c>
+      <c r="AP42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>308799</v>
+        <v>155369</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D43" t="s">
         <v>66</v>
       </c>
       <c r="E43" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K43">
         <v>28000</v>
@@ -3318,29 +3325,38 @@
       <c r="L43">
         <v>130</v>
       </c>
+      <c r="S43">
+        <v>0.75</v>
+      </c>
+      <c r="V43">
+        <v>0.75</v>
+      </c>
       <c r="Y43">
         <v>1</v>
       </c>
       <c r="AA43">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="AB43">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="AC43" t="s">
         <v>66</v>
       </c>
+      <c r="AF43">
+        <v>0.75</v>
+      </c>
       <c r="AL43">
         <v>1</v>
       </c>
-      <c r="BG43">
-        <v>1</v>
-      </c>
-      <c r="BH43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:65">
+      <c r="AM43">
+        <v>1</v>
+      </c>
+      <c r="AP43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>308800</v>
       </c>
@@ -3384,110 +3400,110 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:65">
+    <row r="45" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A45">
+        <v>308802</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>138</v>
+      </c>
+      <c r="K45">
+        <v>40000</v>
+      </c>
+      <c r="L45">
+        <v>180</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Y45">
+        <v>1</v>
+      </c>
+      <c r="AA45">
+        <v>140</v>
+      </c>
+      <c r="AB45">
+        <v>160</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL45">
+        <v>1</v>
+      </c>
+      <c r="AM45">
+        <v>1</v>
+      </c>
+      <c r="AP45">
+        <v>35</v>
+      </c>
+      <c r="AQ45">
+        <v>1</v>
+      </c>
+      <c r="AR45">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:60" x14ac:dyDescent="0.2">
+      <c r="A46">
         <v>308801</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
         <v>136</v>
       </c>
-      <c r="D45" t="s">
-        <v>66</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" t="s">
         <v>132</v>
       </c>
-      <c r="K45">
+      <c r="K46">
         <v>45000</v>
       </c>
-      <c r="L45">
+      <c r="L46">
         <v>200</v>
       </c>
-      <c r="Y45">
-        <v>1</v>
-      </c>
-      <c r="AA45">
+      <c r="Y46">
+        <v>1</v>
+      </c>
+      <c r="AA46">
         <v>160</v>
       </c>
-      <c r="AB45">
+      <c r="AB46">
         <v>170</v>
       </c>
-      <c r="AC45" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL45">
-        <v>1</v>
-      </c>
-      <c r="BG45">
-        <v>1</v>
-      </c>
-      <c r="BH45">
+      <c r="AC46" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL46">
+        <v>1</v>
+      </c>
+      <c r="BG46">
+        <v>1</v>
+      </c>
+      <c r="BH46">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:65">
-      <c r="A46">
-        <v>308802</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E46" t="s">
-        <v>138</v>
-      </c>
-      <c r="K46">
-        <v>40000</v>
-      </c>
-      <c r="L46">
-        <v>180</v>
-      </c>
-      <c r="N46">
-        <v>1</v>
-      </c>
-      <c r="O46">
-        <v>1</v>
-      </c>
-      <c r="P46">
-        <v>1</v>
-      </c>
-      <c r="Y46">
-        <v>1</v>
-      </c>
-      <c r="AA46">
-        <v>140</v>
-      </c>
-      <c r="AB46">
-        <v>160</v>
-      </c>
-      <c r="AC46" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL46">
-        <v>1</v>
-      </c>
-      <c r="AM46">
-        <v>1</v>
-      </c>
-      <c r="AP46">
-        <v>35</v>
-      </c>
-      <c r="AQ46">
-        <v>1</v>
-      </c>
-      <c r="AR46">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:65">
+    <row r="47" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>308803</v>
       </c>
@@ -3561,7 +3577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:65">
+    <row r="48" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>308804</v>
       </c>
@@ -3608,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:65">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>308805</v>
       </c>
@@ -3688,7 +3704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:65">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>308806</v>
       </c>
@@ -3766,18 +3782,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BM50">
+    <sortCondition ref="AA1:AA50"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>